<commit_message>
Added bechmarks of FakeBackends and updated the same in README file
</commit_message>
<xml_diff>
--- a/Qiskit-CPU/Shors/Shor's Order Finding Benchmark-Results.xlsx
+++ b/Qiskit-CPU/Shors/Shor's Order Finding Benchmark-Results.xlsx
@@ -9,6 +9,8 @@
   <sheets>
     <sheet name="qasm_simulator" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="statevector_simulator" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="ibmq_guadalupe-1.2.15" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="fake_guadalupe-1.2.15" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -417,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T23"/>
+  <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1371,7 +1373,6 @@
         <v>4891.08</v>
       </c>
     </row>
-    <row r="23"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A16:S16"/>
@@ -1392,7 +1393,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1428,6 +1429,723 @@
           <t>Qiskit: Algorithm = Shor's Order Finding Simulator = statevector_simulator</t>
         </is>
       </c>
+      <c r="T2" s="1" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>CPU: 12th Gen Intel(R) Core(TM) i9-12900 with 24 cores</t>
+        </is>
+      </c>
+      <c r="T3" s="1" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Configuration: Min_Qubits = 10 Max_Qubits = 25 Skip_Qubits = 4 num_circuits = 2  QV_ = None Last_Updated = 2025-01-20 17:06:54</t>
+        </is>
+      </c>
+      <c r="T4" s="1" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Number of Qubits</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>avg_creation_times (ms)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>std_creation_times (ms)</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>avg_elapsed_times (ms)</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>std_elapsed_times (ms)</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>avg_quantum_times (ms)</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>std_quantum_times (ms)</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>avg_circuit_depths</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>avg_transpiled_depths</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Average_Rescaled_fidelity</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Average_Hellinger_fidelity</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>std_Rescaled_Fidelity</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>std_hellinger_fidelity</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>avg_1Q_algorithmic_gate_counts</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>avg_2Q_algorithmic_gate_counts</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>avg_xi (n2q/n1q+n2q)</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>avg_1Q_Transpiled_gate_counts</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>avg_2Q_Transpiled_gate_counts</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>avg_tr_xi (tr_n2q/tr_n1q+tr_n2q)</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>max_memory (MB)</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>10</v>
+      </c>
+      <c r="B6" t="n">
+        <v>170.155</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2.666</v>
+      </c>
+      <c r="D6" t="n">
+        <v>760.525</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2.554</v>
+      </c>
+      <c r="F6" t="n">
+        <v>561.804</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1.301</v>
+      </c>
+      <c r="H6" t="n">
+        <v>904</v>
+      </c>
+      <c r="I6" t="n">
+        <v>2732</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>101</v>
+      </c>
+      <c r="O6" t="n">
+        <v>106</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>2226</v>
+      </c>
+      <c r="R6" t="n">
+        <v>1644</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="T6" t="n">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>14</v>
+      </c>
+      <c r="B7" t="n">
+        <v>563.476</v>
+      </c>
+      <c r="C7" t="n">
+        <v>8.336</v>
+      </c>
+      <c r="D7" t="n">
+        <v>32455.561</v>
+      </c>
+      <c r="E7" t="n">
+        <v>126.366</v>
+      </c>
+      <c r="F7" t="n">
+        <v>31924.923</v>
+      </c>
+      <c r="G7" t="n">
+        <v>122.238</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2759</v>
+      </c>
+      <c r="I7" t="n">
+        <v>8259.5</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>211</v>
+      </c>
+      <c r="O7" t="n">
+        <v>285</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>6788.5</v>
+      </c>
+      <c r="R7" t="n">
+        <v>5130</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="T7" t="n">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>18</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1227.833</v>
+      </c>
+      <c r="C8" t="n">
+        <v>12.741</v>
+      </c>
+      <c r="D8" t="n">
+        <v>418577.785</v>
+      </c>
+      <c r="E8" t="n">
+        <v>340.93</v>
+      </c>
+      <c r="F8" t="n">
+        <v>417349.223</v>
+      </c>
+      <c r="G8" t="n">
+        <v>333.397</v>
+      </c>
+      <c r="H8" t="n">
+        <v>6478</v>
+      </c>
+      <c r="I8" t="n">
+        <v>19484</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>361</v>
+      </c>
+      <c r="O8" t="n">
+        <v>588</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>15964.5</v>
+      </c>
+      <c r="R8" t="n">
+        <v>12384</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="T8" t="n">
+        <v>1643.45</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>22</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2479.225</v>
+      </c>
+      <c r="C9" t="n">
+        <v>58.466</v>
+      </c>
+      <c r="D9" t="n">
+        <v>13346085.5</v>
+      </c>
+      <c r="E9" t="n">
+        <v>4164.559</v>
+      </c>
+      <c r="F9" t="n">
+        <v>13343574.897</v>
+      </c>
+      <c r="G9" t="n">
+        <v>4186.765</v>
+      </c>
+      <c r="H9" t="n">
+        <v>12997</v>
+      </c>
+      <c r="I9" t="n">
+        <v>38265.5</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1</v>
+      </c>
+      <c r="K9" t="n">
+        <v>1</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>551</v>
+      </c>
+      <c r="O9" t="n">
+        <v>1045</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>30840</v>
+      </c>
+      <c r="R9" t="n">
+        <v>24362</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="T9" t="n">
+        <v>5024.67</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A4:S4"/>
+    <mergeCell ref="A3:S3"/>
+    <mergeCell ref="A2:S2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:T8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr"/>
+      <c r="B1" s="1" t="inlineStr"/>
+      <c r="C1" s="1" t="inlineStr"/>
+      <c r="D1" s="1" t="inlineStr"/>
+      <c r="E1" s="1" t="inlineStr"/>
+      <c r="F1" s="1" t="inlineStr"/>
+      <c r="G1" s="1" t="inlineStr"/>
+      <c r="H1" s="1" t="inlineStr"/>
+      <c r="I1" s="1" t="inlineStr"/>
+      <c r="J1" s="1" t="inlineStr"/>
+      <c r="K1" s="1" t="inlineStr"/>
+      <c r="L1" s="1" t="inlineStr"/>
+      <c r="M1" s="1" t="inlineStr"/>
+      <c r="N1" s="1" t="inlineStr"/>
+      <c r="O1" s="1" t="inlineStr"/>
+      <c r="P1" s="1" t="inlineStr"/>
+      <c r="Q1" s="1" t="inlineStr"/>
+      <c r="R1" s="1" t="inlineStr"/>
+      <c r="S1" s="1" t="inlineStr"/>
+      <c r="T1" s="1" t="inlineStr"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Qiskit: Algorithm = Shor's Order Finding Simulator = ibmq_guadalupe-1.2.15</t>
+        </is>
+      </c>
+      <c r="T2" s="1" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>CPU: 12th Gen Intel(R) Core(TM) i9-12900 with 24 cores</t>
+        </is>
+      </c>
+      <c r="T3" s="1" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Configuration: Min_Qubits = 10 Max_Qubits = 16 Skip_Qubits = 4 num_circuits = 2  QV_ = 32 Last_Updated = 2025-02-11 12:20:32</t>
+        </is>
+      </c>
+      <c r="T4" s="1" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Number of Qubits</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>avg_creation_times (ms)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>std_creation_times (ms)</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>avg_elapsed_times (ms)</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>std_elapsed_times (ms)</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>avg_quantum_times (ms)</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>std_quantum_times (ms)</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>avg_circuit_depths</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>avg_transpiled_depths</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Average_Rescaled_fidelity</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Average_Hellinger_fidelity</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>std_Rescaled_Fidelity</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>std_hellinger_fidelity</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>avg_1Q_algorithmic_gate_counts</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>avg_2Q_algorithmic_gate_counts</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>avg_xi (n2q/n1q+n2q)</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>avg_1Q_Transpiled_gate_counts</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>avg_2Q_Transpiled_gate_counts</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>avg_tr_xi (tr_n2q/tr_n1q+tr_n2q)</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>max_memory (MB)</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>10</v>
+      </c>
+      <c r="B6" t="n">
+        <v>213.62</v>
+      </c>
+      <c r="C6" t="n">
+        <v>10.245</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3748.484</v>
+      </c>
+      <c r="E6" t="n">
+        <v>28.662</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3642.925</v>
+      </c>
+      <c r="G6" t="n">
+        <v>23.067</v>
+      </c>
+      <c r="H6" t="n">
+        <v>904</v>
+      </c>
+      <c r="I6" t="n">
+        <v>5027.5</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.018</v>
+      </c>
+      <c r="N6" t="n">
+        <v>101</v>
+      </c>
+      <c r="O6" t="n">
+        <v>106</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>2531</v>
+      </c>
+      <c r="R6" t="n">
+        <v>3759</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="T6" t="n">
+        <v>291.42</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>14</v>
+      </c>
+      <c r="B7" t="n">
+        <v>550.847</v>
+      </c>
+      <c r="C7" t="n">
+        <v>6.62</v>
+      </c>
+      <c r="D7" t="n">
+        <v>743365.202</v>
+      </c>
+      <c r="E7" t="n">
+        <v>246136.731</v>
+      </c>
+      <c r="F7" t="n">
+        <v>743361.142</v>
+      </c>
+      <c r="G7" t="n">
+        <v>246136.269</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2759</v>
+      </c>
+      <c r="I7" t="n">
+        <v>15843.5</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="N7" t="n">
+        <v>211</v>
+      </c>
+      <c r="O7" t="n">
+        <v>285</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>7605.5</v>
+      </c>
+      <c r="R7" t="n">
+        <v>12960</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="T7" t="n">
+        <v>5478.98</v>
+      </c>
+    </row>
+    <row r="8"/>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A4:S4"/>
+    <mergeCell ref="A3:S3"/>
+    <mergeCell ref="A2:S2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:T8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr"/>
+      <c r="B1" s="1" t="inlineStr"/>
+      <c r="C1" s="1" t="inlineStr"/>
+      <c r="D1" s="1" t="inlineStr"/>
+      <c r="E1" s="1" t="inlineStr"/>
+      <c r="F1" s="1" t="inlineStr"/>
+      <c r="G1" s="1" t="inlineStr"/>
+      <c r="H1" s="1" t="inlineStr"/>
+      <c r="I1" s="1" t="inlineStr"/>
+      <c r="J1" s="1" t="inlineStr"/>
+      <c r="K1" s="1" t="inlineStr"/>
+      <c r="L1" s="1" t="inlineStr"/>
+      <c r="M1" s="1" t="inlineStr"/>
+      <c r="N1" s="1" t="inlineStr"/>
+      <c r="O1" s="1" t="inlineStr"/>
+      <c r="P1" s="1" t="inlineStr"/>
+      <c r="Q1" s="1" t="inlineStr"/>
+      <c r="R1" s="1" t="inlineStr"/>
+      <c r="S1" s="1" t="inlineStr"/>
+      <c r="T1" s="1" t="inlineStr"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Qiskit: Algorithm = Shor's Order Finding Simulator = fake_guadalupe-1.2.15</t>
+        </is>
+      </c>
       <c r="B2" s="1" t="n"/>
       <c r="C2" s="1" t="n"/>
       <c r="D2" s="1" t="n"/>
@@ -1477,7 +2195,7 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Configuration: Min_Qubits = 10 Max_Qubits = 25 Skip_Qubits = 4 num_circuits = 2  QV_ = None Last_Updated = 2025-01-20 17:06:54</t>
+          <t>Configuration: Min_Qubits = 10 Max_Qubits = 16 Skip_Qubits = 4 num_circuits = 2  QV_ = 32 Last_Updated = 2025-02-11 12:41:02</t>
         </is>
       </c>
       <c r="B4" s="1" t="n"/>
@@ -1607,40 +2325,40 @@
         <v>10</v>
       </c>
       <c r="B6" t="n">
-        <v>170.155</v>
+        <v>187.321</v>
       </c>
       <c r="C6" t="n">
-        <v>2.666</v>
+        <v>8.308</v>
       </c>
       <c r="D6" t="n">
-        <v>760.525</v>
+        <v>39139.159</v>
       </c>
       <c r="E6" t="n">
-        <v>2.554</v>
+        <v>16978.188</v>
       </c>
       <c r="F6" t="n">
-        <v>561.804</v>
+        <v>39061.794</v>
       </c>
       <c r="G6" t="n">
-        <v>1.301</v>
+        <v>16940.393</v>
       </c>
       <c r="H6" t="n">
         <v>904</v>
       </c>
       <c r="I6" t="n">
-        <v>2732</v>
+        <v>4967</v>
       </c>
       <c r="J6" t="n">
-        <v>1</v>
+        <v>0.02</v>
       </c>
       <c r="K6" t="n">
-        <v>1</v>
+        <v>0.15</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>0.007</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>0.006</v>
       </c>
       <c r="N6" t="n">
         <v>101</v>
@@ -1652,16 +2370,16 @@
         <v>0.51</v>
       </c>
       <c r="Q6" t="n">
-        <v>2226</v>
+        <v>2530</v>
       </c>
       <c r="R6" t="n">
-        <v>1644</v>
+        <v>3787</v>
       </c>
       <c r="S6" t="n">
-        <v>0.42</v>
+        <v>0.6</v>
       </c>
       <c r="T6" t="n">
-        <v>833</v>
+        <v>308.97</v>
       </c>
     </row>
     <row r="7">
@@ -1669,40 +2387,40 @@
         <v>14</v>
       </c>
       <c r="B7" t="n">
-        <v>563.476</v>
+        <v>585.341</v>
       </c>
       <c r="C7" t="n">
-        <v>8.336</v>
+        <v>6.859</v>
       </c>
       <c r="D7" t="n">
-        <v>32455.561</v>
+        <v>182217.006</v>
       </c>
       <c r="E7" t="n">
-        <v>126.366</v>
+        <v>1710.004</v>
       </c>
       <c r="F7" t="n">
-        <v>31924.923</v>
+        <v>182212.26</v>
       </c>
       <c r="G7" t="n">
-        <v>122.238</v>
+        <v>1709.506</v>
       </c>
       <c r="H7" t="n">
         <v>2759</v>
       </c>
       <c r="I7" t="n">
-        <v>8259.5</v>
+        <v>16040</v>
       </c>
       <c r="J7" t="n">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="K7" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
+        <v>0.004</v>
       </c>
       <c r="M7" t="n">
-        <v>0</v>
+        <v>0.004</v>
       </c>
       <c r="N7" t="n">
         <v>211</v>
@@ -1714,163 +2432,39 @@
         <v>0.57</v>
       </c>
       <c r="Q7" t="n">
-        <v>6788.5</v>
+        <v>7602</v>
       </c>
       <c r="R7" t="n">
-        <v>5130</v>
+        <v>13346</v>
       </c>
       <c r="S7" t="n">
-        <v>0.43</v>
+        <v>0.64</v>
       </c>
       <c r="T7" t="n">
-        <v>833</v>
+        <v>497.26</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>18</v>
-      </c>
-      <c r="B8" t="n">
-        <v>1227.833</v>
-      </c>
-      <c r="C8" t="n">
-        <v>12.741</v>
-      </c>
-      <c r="D8" t="n">
-        <v>418577.785</v>
-      </c>
-      <c r="E8" t="n">
-        <v>340.93</v>
-      </c>
-      <c r="F8" t="n">
-        <v>417349.223</v>
-      </c>
-      <c r="G8" t="n">
-        <v>333.397</v>
-      </c>
-      <c r="H8" t="n">
-        <v>6478</v>
-      </c>
-      <c r="I8" t="n">
-        <v>19484</v>
-      </c>
-      <c r="J8" t="n">
-        <v>1</v>
-      </c>
-      <c r="K8" t="n">
-        <v>1</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0</v>
-      </c>
-      <c r="N8" t="n">
-        <v>361</v>
-      </c>
-      <c r="O8" t="n">
-        <v>588</v>
-      </c>
-      <c r="P8" t="n">
-        <v>0.62</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>15964.5</v>
-      </c>
-      <c r="R8" t="n">
-        <v>12384</v>
-      </c>
-      <c r="S8" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="T8" t="n">
-        <v>1643.45</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>22</v>
-      </c>
-      <c r="B9" t="n">
-        <v>2479.225</v>
-      </c>
-      <c r="C9" t="n">
-        <v>58.466</v>
-      </c>
-      <c r="D9" t="n">
-        <v>13346085.5</v>
-      </c>
-      <c r="E9" t="n">
-        <v>4164.559</v>
-      </c>
-      <c r="F9" t="n">
-        <v>13343574.897</v>
-      </c>
-      <c r="G9" t="n">
-        <v>4186.765</v>
-      </c>
-      <c r="H9" t="n">
-        <v>12997</v>
-      </c>
-      <c r="I9" t="n">
-        <v>38265.5</v>
-      </c>
-      <c r="J9" t="n">
-        <v>1</v>
-      </c>
-      <c r="K9" t="n">
-        <v>1</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N9" t="n">
-        <v>551</v>
-      </c>
-      <c r="O9" t="n">
-        <v>1045</v>
-      </c>
-      <c r="P9" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>30840</v>
-      </c>
-      <c r="R9" t="n">
-        <v>24362</v>
-      </c>
-      <c r="S9" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="T9" t="n">
-        <v>5024.67</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" t="inlineStr"/>
-      <c r="T10" t="inlineStr"/>
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr"/>
+      <c r="T8" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Performed Benchmarks for Method-2 of Shors
</commit_message>
<xml_diff>
--- a/Qiskit-CPU/Shors/Shor's Order Finding Benchmark-Results.xlsx
+++ b/Qiskit-CPU/Shors/Shor's Order Finding Benchmark-Results.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T22"/>
+  <dimension ref="A1:T47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1024,362 +1024,1440 @@
       <c r="T17" s="1" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" s="1" t="inlineStr">
         <is>
           <t>Number of Qubits</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B18" s="1" t="inlineStr">
         <is>
           <t>avg_creation_times (ms)</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C18" s="1" t="inlineStr">
         <is>
           <t>std_creation_times (ms)</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="D18" s="1" t="inlineStr">
         <is>
           <t>avg_elapsed_times (ms)</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="E18" s="1" t="inlineStr">
         <is>
           <t>std_elapsed_times (ms)</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="F18" s="1" t="inlineStr">
         <is>
           <t>avg_quantum_times (ms)</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="G18" s="1" t="inlineStr">
         <is>
           <t>std_quantum_times (ms)</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
+      <c r="H18" s="1" t="inlineStr">
         <is>
           <t>avg_circuit_depths</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr">
+      <c r="I18" s="1" t="inlineStr">
         <is>
           <t>avg_transpiled_depths</t>
         </is>
       </c>
-      <c r="J18" t="inlineStr">
+      <c r="J18" s="1" t="inlineStr">
         <is>
           <t>Average_Rescaled_fidelity</t>
         </is>
       </c>
-      <c r="K18" t="inlineStr">
+      <c r="K18" s="1" t="inlineStr">
         <is>
           <t>Average_Hellinger_fidelity</t>
         </is>
       </c>
-      <c r="L18" t="inlineStr">
+      <c r="L18" s="1" t="inlineStr">
         <is>
           <t>std_Rescaled_Fidelity</t>
         </is>
       </c>
-      <c r="M18" t="inlineStr">
+      <c r="M18" s="1" t="inlineStr">
         <is>
           <t>std_hellinger_fidelity</t>
         </is>
       </c>
-      <c r="N18" t="inlineStr">
+      <c r="N18" s="1" t="inlineStr">
         <is>
           <t>avg_1Q_algorithmic_gate_counts</t>
         </is>
       </c>
-      <c r="O18" t="inlineStr">
+      <c r="O18" s="1" t="inlineStr">
         <is>
           <t>avg_2Q_algorithmic_gate_counts</t>
         </is>
       </c>
-      <c r="P18" t="inlineStr">
+      <c r="P18" s="1" t="inlineStr">
         <is>
           <t>avg_xi (n2q/n1q+n2q)</t>
         </is>
       </c>
-      <c r="Q18" t="inlineStr">
+      <c r="Q18" s="1" t="inlineStr">
         <is>
           <t>avg_1Q_Transpiled_gate_counts</t>
         </is>
       </c>
-      <c r="R18" t="inlineStr">
+      <c r="R18" s="1" t="inlineStr">
         <is>
           <t>avg_2Q_Transpiled_gate_counts</t>
         </is>
       </c>
-      <c r="S18" t="inlineStr">
+      <c r="S18" s="1" t="inlineStr">
         <is>
           <t>avg_tr_xi (tr_n2q/tr_n1q+tr_n2q)</t>
         </is>
       </c>
-      <c r="T18" t="inlineStr">
+      <c r="T18" s="1" t="inlineStr">
         <is>
           <t>max_memory (MB)</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
+      <c r="A19" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B19" t="n">
+      <c r="B19" s="1" t="n">
         <v>187.328</v>
       </c>
-      <c r="C19" t="n">
+      <c r="C19" s="1" t="n">
         <v>3.795</v>
       </c>
-      <c r="D19" t="n">
+      <c r="D19" s="1" t="n">
         <v>2151.056</v>
       </c>
-      <c r="E19" t="n">
+      <c r="E19" s="1" t="n">
         <v>15.215</v>
       </c>
-      <c r="F19" t="n">
+      <c r="F19" s="1" t="n">
         <v>1937.952</v>
       </c>
-      <c r="G19" t="n">
+      <c r="G19" s="1" t="n">
         <v>13.149</v>
       </c>
-      <c r="H19" t="n">
+      <c r="H19" s="1" t="n">
         <v>904</v>
       </c>
-      <c r="I19" t="n">
+      <c r="I19" s="1" t="n">
         <v>2732</v>
       </c>
-      <c r="J19" t="n">
+      <c r="J19" s="1" t="n">
         <v>0.01</v>
       </c>
-      <c r="K19" t="n">
+      <c r="K19" s="1" t="n">
         <v>0.13</v>
       </c>
-      <c r="L19" t="n">
+      <c r="L19" s="1" t="n">
         <v>0.003</v>
       </c>
-      <c r="M19" t="n">
+      <c r="M19" s="1" t="n">
         <v>0.004</v>
       </c>
-      <c r="N19" t="n">
+      <c r="N19" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="O19" t="n">
+      <c r="O19" s="1" t="n">
         <v>106</v>
       </c>
-      <c r="P19" t="n">
+      <c r="P19" s="1" t="n">
         <v>0.51</v>
       </c>
-      <c r="Q19" t="n">
+      <c r="Q19" s="1" t="n">
         <v>2226</v>
       </c>
-      <c r="R19" t="n">
+      <c r="R19" s="1" t="n">
         <v>1644</v>
       </c>
-      <c r="S19" t="n">
+      <c r="S19" s="1" t="n">
         <v>0.42</v>
       </c>
-      <c r="T19" t="n">
+      <c r="T19" s="1" t="n">
         <v>832.09</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
+      <c r="A20" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B20" t="n">
+      <c r="B20" s="1" t="n">
         <v>577.139</v>
       </c>
-      <c r="C20" t="n">
+      <c r="C20" s="1" t="n">
         <v>8.817</v>
       </c>
-      <c r="D20" t="n">
+      <c r="D20" s="1" t="n">
         <v>36479.131</v>
       </c>
-      <c r="E20" t="n">
+      <c r="E20" s="1" t="n">
         <v>229.871</v>
       </c>
-      <c r="F20" t="n">
+      <c r="F20" s="1" t="n">
         <v>35896.515</v>
       </c>
-      <c r="G20" t="n">
+      <c r="G20" s="1" t="n">
         <v>222.296</v>
       </c>
-      <c r="H20" t="n">
+      <c r="H20" s="1" t="n">
         <v>2759</v>
       </c>
-      <c r="I20" t="n">
+      <c r="I20" s="1" t="n">
         <v>8259.5</v>
       </c>
-      <c r="J20" t="n">
-        <v>0</v>
-      </c>
-      <c r="K20" t="n">
+      <c r="J20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1" t="n">
         <v>0.03</v>
       </c>
-      <c r="L20" t="n">
+      <c r="L20" s="1" t="n">
         <v>0.001</v>
       </c>
-      <c r="M20" t="n">
+      <c r="M20" s="1" t="n">
         <v>0.001</v>
       </c>
-      <c r="N20" t="n">
+      <c r="N20" s="1" t="n">
         <v>211</v>
       </c>
-      <c r="O20" t="n">
+      <c r="O20" s="1" t="n">
         <v>285</v>
       </c>
-      <c r="P20" t="n">
+      <c r="P20" s="1" t="n">
         <v>0.57</v>
       </c>
-      <c r="Q20" t="n">
+      <c r="Q20" s="1" t="n">
         <v>6788.5</v>
       </c>
-      <c r="R20" t="n">
+      <c r="R20" s="1" t="n">
         <v>5130</v>
       </c>
-      <c r="S20" t="n">
+      <c r="S20" s="1" t="n">
         <v>0.43</v>
       </c>
-      <c r="T20" t="n">
+      <c r="T20" s="1" t="n">
         <v>933.62</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
+      <c r="A21" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B21" t="n">
+      <c r="B21" s="1" t="n">
         <v>1251.722</v>
       </c>
-      <c r="C21" t="n">
+      <c r="C21" s="1" t="n">
         <v>14.818</v>
       </c>
-      <c r="D21" t="n">
+      <c r="D21" s="1" t="n">
         <v>479711.638</v>
       </c>
-      <c r="E21" t="n">
+      <c r="E21" s="1" t="n">
         <v>634.306</v>
       </c>
-      <c r="F21" t="n">
+      <c r="F21" s="1" t="n">
         <v>478208.315</v>
       </c>
-      <c r="G21" t="n">
+      <c r="G21" s="1" t="n">
         <v>582.741</v>
       </c>
-      <c r="H21" t="n">
+      <c r="H21" s="1" t="n">
         <v>6478</v>
       </c>
-      <c r="I21" t="n">
+      <c r="I21" s="1" t="n">
         <v>19484</v>
       </c>
-      <c r="J21" t="n">
-        <v>0</v>
-      </c>
-      <c r="K21" t="n">
+      <c r="J21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" s="1" t="n">
         <v>0.01</v>
       </c>
-      <c r="L21" t="n">
-        <v>0</v>
-      </c>
-      <c r="M21" t="n">
-        <v>0</v>
-      </c>
-      <c r="N21" t="n">
+      <c r="L21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" s="1" t="n">
         <v>361</v>
       </c>
-      <c r="O21" t="n">
+      <c r="O21" s="1" t="n">
         <v>588</v>
       </c>
-      <c r="P21" t="n">
+      <c r="P21" s="1" t="n">
         <v>0.62</v>
       </c>
-      <c r="Q21" t="n">
+      <c r="Q21" s="1" t="n">
         <v>15964.5</v>
       </c>
-      <c r="R21" t="n">
+      <c r="R21" s="1" t="n">
         <v>12384</v>
       </c>
-      <c r="S21" t="n">
+      <c r="S21" s="1" t="n">
         <v>0.44</v>
       </c>
-      <c r="T21" t="n">
+      <c r="T21" s="1" t="n">
         <v>1875.6</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="n">
+      <c r="A22" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B22" t="n">
+      <c r="B22" s="1" t="n">
         <v>2455.598</v>
       </c>
-      <c r="C22" t="n">
+      <c r="C22" s="1" t="n">
         <v>18.279</v>
       </c>
-      <c r="D22" t="n">
+      <c r="D22" s="1" t="n">
         <v>15759371.525</v>
       </c>
-      <c r="E22" t="n">
+      <c r="E22" s="1" t="n">
         <v>1760.002</v>
       </c>
-      <c r="F22" t="n">
+      <c r="F22" s="1" t="n">
         <v>15756634.916</v>
       </c>
-      <c r="G22" t="n">
+      <c r="G22" s="1" t="n">
         <v>1739.585</v>
       </c>
-      <c r="H22" t="n">
+      <c r="H22" s="1" t="n">
         <v>12997</v>
       </c>
-      <c r="I22" t="n">
+      <c r="I22" s="1" t="n">
         <v>38265.5</v>
       </c>
-      <c r="J22" t="n">
-        <v>0</v>
-      </c>
-      <c r="K22" t="n">
-        <v>0</v>
-      </c>
-      <c r="L22" t="n">
-        <v>0</v>
-      </c>
-      <c r="M22" t="n">
-        <v>0</v>
-      </c>
-      <c r="N22" t="n">
+      <c r="J22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N22" s="1" t="n">
         <v>551</v>
       </c>
-      <c r="O22" t="n">
+      <c r="O22" s="1" t="n">
         <v>1045</v>
       </c>
-      <c r="P22" t="n">
+      <c r="P22" s="1" t="n">
         <v>0.65</v>
       </c>
-      <c r="Q22" t="n">
+      <c r="Q22" s="1" t="n">
         <v>30840</v>
       </c>
-      <c r="R22" t="n">
+      <c r="R22" s="1" t="n">
         <v>24362</v>
       </c>
-      <c r="S22" t="n">
+      <c r="S22" s="1" t="n">
         <v>0.44</v>
       </c>
-      <c r="T22" t="n">
+      <c r="T22" s="1" t="n">
         <v>4891.08</v>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr"/>
+      <c r="B23" s="1" t="inlineStr"/>
+      <c r="C23" s="1" t="inlineStr"/>
+      <c r="D23" s="1" t="inlineStr"/>
+      <c r="E23" s="1" t="inlineStr"/>
+      <c r="F23" s="1" t="inlineStr"/>
+      <c r="G23" s="1" t="inlineStr"/>
+      <c r="H23" s="1" t="inlineStr"/>
+      <c r="I23" s="1" t="inlineStr"/>
+      <c r="J23" s="1" t="inlineStr"/>
+      <c r="K23" s="1" t="inlineStr"/>
+      <c r="L23" s="1" t="inlineStr"/>
+      <c r="M23" s="1" t="inlineStr"/>
+      <c r="N23" s="1" t="inlineStr"/>
+      <c r="O23" s="1" t="inlineStr"/>
+      <c r="P23" s="1" t="inlineStr"/>
+      <c r="Q23" s="1" t="inlineStr"/>
+      <c r="R23" s="1" t="inlineStr"/>
+      <c r="S23" s="1" t="inlineStr"/>
+      <c r="T23" s="1" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>Qiskit: Algorithm = Shor's Order Finding Simulator = qasm_simulator</t>
+        </is>
+      </c>
+      <c r="T24" s="1" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>CPU: 12th Gen Intel(R) Core(TM) i9-12900 with 24 cores</t>
+        </is>
+      </c>
+      <c r="T25" s="1" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>Configuration: Min_Qubits = 7 Max_Qubits = 17 Skip_Qubits = 2 num_circuits = 2  QV_ = None Last_Updated = 2025-02-11 15:15:32</t>
+        </is>
+      </c>
+      <c r="T26" s="1" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>Number of Qubits</t>
+        </is>
+      </c>
+      <c r="B27" s="1" t="inlineStr">
+        <is>
+          <t>avg_creation_times (ms)</t>
+        </is>
+      </c>
+      <c r="C27" s="1" t="inlineStr">
+        <is>
+          <t>std_creation_times (ms)</t>
+        </is>
+      </c>
+      <c r="D27" s="1" t="inlineStr">
+        <is>
+          <t>avg_elapsed_times (ms)</t>
+        </is>
+      </c>
+      <c r="E27" s="1" t="inlineStr">
+        <is>
+          <t>std_elapsed_times (ms)</t>
+        </is>
+      </c>
+      <c r="F27" s="1" t="inlineStr">
+        <is>
+          <t>avg_quantum_times (ms)</t>
+        </is>
+      </c>
+      <c r="G27" s="1" t="inlineStr">
+        <is>
+          <t>std_quantum_times (ms)</t>
+        </is>
+      </c>
+      <c r="H27" s="1" t="inlineStr">
+        <is>
+          <t>avg_circuit_depths</t>
+        </is>
+      </c>
+      <c r="I27" s="1" t="inlineStr">
+        <is>
+          <t>avg_transpiled_depths</t>
+        </is>
+      </c>
+      <c r="J27" s="1" t="inlineStr">
+        <is>
+          <t>Average_Rescaled_fidelity</t>
+        </is>
+      </c>
+      <c r="K27" s="1" t="inlineStr">
+        <is>
+          <t>Average_Hellinger_fidelity</t>
+        </is>
+      </c>
+      <c r="L27" s="1" t="inlineStr">
+        <is>
+          <t>std_Rescaled_Fidelity</t>
+        </is>
+      </c>
+      <c r="M27" s="1" t="inlineStr">
+        <is>
+          <t>std_hellinger_fidelity</t>
+        </is>
+      </c>
+      <c r="N27" s="1" t="inlineStr">
+        <is>
+          <t>avg_1Q_algorithmic_gate_counts</t>
+        </is>
+      </c>
+      <c r="O27" s="1" t="inlineStr">
+        <is>
+          <t>avg_2Q_algorithmic_gate_counts</t>
+        </is>
+      </c>
+      <c r="P27" s="1" t="inlineStr">
+        <is>
+          <t>avg_xi (n2q/n1q+n2q)</t>
+        </is>
+      </c>
+      <c r="Q27" s="1" t="inlineStr">
+        <is>
+          <t>avg_1Q_Transpiled_gate_counts</t>
+        </is>
+      </c>
+      <c r="R27" s="1" t="inlineStr">
+        <is>
+          <t>avg_2Q_Transpiled_gate_counts</t>
+        </is>
+      </c>
+      <c r="S27" s="1" t="inlineStr">
+        <is>
+          <t>avg_tr_xi (tr_n2q/tr_n1q+tr_n2q)</t>
+        </is>
+      </c>
+      <c r="T27" s="1" t="inlineStr">
+        <is>
+          <t>max_memory (MB)</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B28" s="1" t="n">
+        <v>202.636</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>10.958</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <v>294.857</v>
+      </c>
+      <c r="E28" s="1" t="n">
+        <v>10.541</v>
+      </c>
+      <c r="F28" s="1" t="n">
+        <v>120.862</v>
+      </c>
+      <c r="G28" s="1" t="n">
+        <v>1.617</v>
+      </c>
+      <c r="H28" s="1" t="n">
+        <v>881</v>
+      </c>
+      <c r="I28" s="1" t="n">
+        <v>2752</v>
+      </c>
+      <c r="J28" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K28" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="O28" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="P28" s="1" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="Q28" s="1" t="n">
+        <v>2321</v>
+      </c>
+      <c r="R28" s="1" t="n">
+        <v>1632</v>
+      </c>
+      <c r="S28" s="1" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="T28" s="1" t="n">
+        <v>213.46</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B29" s="1" t="n">
+        <v>584.973</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>6.548</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>1296.385</v>
+      </c>
+      <c r="E29" s="1" t="n">
+        <v>0.871</v>
+      </c>
+      <c r="F29" s="1" t="n">
+        <v>871.009</v>
+      </c>
+      <c r="G29" s="1" t="n">
+        <v>1.497</v>
+      </c>
+      <c r="H29" s="1" t="n">
+        <v>2720</v>
+      </c>
+      <c r="I29" s="1" t="n">
+        <v>8431.5</v>
+      </c>
+      <c r="J29" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K29" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N29" s="1" t="n">
+        <v>268</v>
+      </c>
+      <c r="O29" s="1" t="n">
+        <v>216</v>
+      </c>
+      <c r="P29" s="1" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="Q29" s="1" t="n">
+        <v>7123.5</v>
+      </c>
+      <c r="R29" s="1" t="n">
+        <v>5100</v>
+      </c>
+      <c r="S29" s="1" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="T29" s="1" t="n">
+        <v>304.16</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B30" s="1" t="n">
+        <v>1180.372</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>12.651</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <v>10148.657</v>
+      </c>
+      <c r="E30" s="1" t="n">
+        <v>239.583</v>
+      </c>
+      <c r="F30" s="1" t="n">
+        <v>8981.732</v>
+      </c>
+      <c r="G30" s="1" t="n">
+        <v>234.259</v>
+      </c>
+      <c r="H30" s="1" t="n">
+        <v>6513</v>
+      </c>
+      <c r="I30" s="1" t="n">
+        <v>20465</v>
+      </c>
+      <c r="J30" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K30" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N30" s="1" t="n">
+        <v>600</v>
+      </c>
+      <c r="O30" s="1" t="n">
+        <v>416</v>
+      </c>
+      <c r="P30" s="1" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="Q30" s="1" t="n">
+        <v>17251.5</v>
+      </c>
+      <c r="R30" s="1" t="n">
+        <v>12328</v>
+      </c>
+      <c r="S30" s="1" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="T30" s="1" t="n">
+        <v>455.16</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B31" s="1" t="n">
+        <v>2219.384</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>4.568</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <v>75010.23299999999</v>
+      </c>
+      <c r="E31" s="1" t="n">
+        <v>201.282</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <v>72533.518</v>
+      </c>
+      <c r="G31" s="1" t="n">
+        <v>197.122</v>
+      </c>
+      <c r="H31" s="1" t="n">
+        <v>13619</v>
+      </c>
+      <c r="I31" s="1" t="n">
+        <v>42860.5</v>
+      </c>
+      <c r="J31" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K31" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N31" s="1" t="n">
+        <v>1544</v>
+      </c>
+      <c r="O31" s="1" t="n">
+        <v>700</v>
+      </c>
+      <c r="P31" s="1" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="Q31" s="1" t="n">
+        <v>35951</v>
+      </c>
+      <c r="R31" s="1" t="n">
+        <v>24272</v>
+      </c>
+      <c r="S31" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="T31" s="1" t="n">
+        <v>688.36</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B32" s="1" t="n">
+        <v>4021.952</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>53.012</v>
+      </c>
+      <c r="D32" s="1" t="n">
+        <v>204894.747</v>
+      </c>
+      <c r="E32" s="1" t="n">
+        <v>2443.179</v>
+      </c>
+      <c r="F32" s="1" t="n">
+        <v>200123.39</v>
+      </c>
+      <c r="G32" s="1" t="n">
+        <v>2496.944</v>
+      </c>
+      <c r="H32" s="1" t="n">
+        <v>26866</v>
+      </c>
+      <c r="I32" s="1" t="n">
+        <v>91280</v>
+      </c>
+      <c r="J32" s="1" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="K32" s="1" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="L32" s="1" t="n">
+        <v>0.166</v>
+      </c>
+      <c r="M32" s="1" t="n">
+        <v>0.166</v>
+      </c>
+      <c r="N32" s="1" t="n">
+        <v>4828</v>
+      </c>
+      <c r="O32" s="1" t="n">
+        <v>1080</v>
+      </c>
+      <c r="P32" s="1" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="Q32" s="1" t="n">
+        <v>78034.5</v>
+      </c>
+      <c r="R32" s="1" t="n">
+        <v>46296</v>
+      </c>
+      <c r="S32" s="1" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="T32" s="1" t="n">
+        <v>1130.2</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B33" s="1" t="n">
+        <v>6888.425</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>27.395</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>1279571.48</v>
+      </c>
+      <c r="E33" s="1" t="n">
+        <v>1101.598</v>
+      </c>
+      <c r="F33" s="1" t="n">
+        <v>1270095.318</v>
+      </c>
+      <c r="G33" s="1" t="n">
+        <v>942.058</v>
+      </c>
+      <c r="H33" s="1" t="n">
+        <v>54484</v>
+      </c>
+      <c r="I33" s="1" t="n">
+        <v>196438</v>
+      </c>
+      <c r="J33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" s="1" t="n">
+        <v>17364</v>
+      </c>
+      <c r="O33" s="1" t="n">
+        <v>1568</v>
+      </c>
+      <c r="P33" s="1" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="Q33" s="1" t="n">
+        <v>173693</v>
+      </c>
+      <c r="R33" s="1" t="n">
+        <v>74788</v>
+      </c>
+      <c r="S33" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="T33" s="1" t="n">
+        <v>1994.57</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr"/>
+      <c r="B34" s="1" t="inlineStr"/>
+      <c r="C34" s="1" t="inlineStr"/>
+      <c r="D34" s="1" t="inlineStr"/>
+      <c r="E34" s="1" t="inlineStr"/>
+      <c r="F34" s="1" t="inlineStr"/>
+      <c r="G34" s="1" t="inlineStr"/>
+      <c r="H34" s="1" t="inlineStr"/>
+      <c r="I34" s="1" t="inlineStr"/>
+      <c r="J34" s="1" t="inlineStr"/>
+      <c r="K34" s="1" t="inlineStr"/>
+      <c r="L34" s="1" t="inlineStr"/>
+      <c r="M34" s="1" t="inlineStr"/>
+      <c r="N34" s="1" t="inlineStr"/>
+      <c r="O34" s="1" t="inlineStr"/>
+      <c r="P34" s="1" t="inlineStr"/>
+      <c r="Q34" s="1" t="inlineStr"/>
+      <c r="R34" s="1" t="inlineStr"/>
+      <c r="S34" s="1" t="inlineStr"/>
+      <c r="T34" s="1" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr"/>
+      <c r="B35" s="1" t="inlineStr"/>
+      <c r="C35" s="1" t="inlineStr"/>
+      <c r="D35" s="1" t="inlineStr"/>
+      <c r="E35" s="1" t="inlineStr"/>
+      <c r="F35" s="1" t="inlineStr"/>
+      <c r="G35" s="1" t="inlineStr"/>
+      <c r="H35" s="1" t="inlineStr"/>
+      <c r="I35" s="1" t="inlineStr"/>
+      <c r="J35" s="1" t="inlineStr"/>
+      <c r="K35" s="1" t="inlineStr"/>
+      <c r="L35" s="1" t="inlineStr"/>
+      <c r="M35" s="1" t="inlineStr"/>
+      <c r="N35" s="1" t="inlineStr"/>
+      <c r="O35" s="1" t="inlineStr"/>
+      <c r="P35" s="1" t="inlineStr"/>
+      <c r="Q35" s="1" t="inlineStr"/>
+      <c r="R35" s="1" t="inlineStr"/>
+      <c r="S35" s="1" t="inlineStr"/>
+      <c r="T35" s="1" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>Qiskit: Algorithm = Shor's Order Finding Simulator = qasm_simulator</t>
+        </is>
+      </c>
+      <c r="T36" s="1" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>CPU: 12th Gen Intel(R) Core(TM) i9-12900 with 24 cores</t>
+        </is>
+      </c>
+      <c r="T37" s="1" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>Executing with Noise</t>
+        </is>
+      </c>
+      <c r="T38" s="1" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>Configuration: Min_Qubits = 7 Max_Qubits = 17 Skip_Qubits = 2 num_circuits = 2  QV_ = None Last_Updated = 2025-02-11 17:02:48</t>
+        </is>
+      </c>
+      <c r="T39" s="1" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Number of Qubits</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>avg_creation_times (ms)</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>std_creation_times (ms)</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>avg_elapsed_times (ms)</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>std_elapsed_times (ms)</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>avg_quantum_times (ms)</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>std_quantum_times (ms)</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>avg_circuit_depths</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>avg_transpiled_depths</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>Average_Rescaled_fidelity</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>Average_Hellinger_fidelity</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>std_Rescaled_Fidelity</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>std_hellinger_fidelity</t>
+        </is>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>avg_1Q_algorithmic_gate_counts</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>avg_2Q_algorithmic_gate_counts</t>
+        </is>
+      </c>
+      <c r="P40" t="inlineStr">
+        <is>
+          <t>avg_xi (n2q/n1q+n2q)</t>
+        </is>
+      </c>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>avg_1Q_Transpiled_gate_counts</t>
+        </is>
+      </c>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>avg_2Q_Transpiled_gate_counts</t>
+        </is>
+      </c>
+      <c r="S40" t="inlineStr">
+        <is>
+          <t>avg_tr_xi (tr_n2q/tr_n1q+tr_n2q)</t>
+        </is>
+      </c>
+      <c r="T40" t="inlineStr">
+        <is>
+          <t>max_memory (MB)</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>7</v>
+      </c>
+      <c r="B41" t="n">
+        <v>198.31</v>
+      </c>
+      <c r="C41" t="n">
+        <v>9.831</v>
+      </c>
+      <c r="D41" t="n">
+        <v>1232.159</v>
+      </c>
+      <c r="E41" t="n">
+        <v>6.945</v>
+      </c>
+      <c r="F41" t="n">
+        <v>1090.377</v>
+      </c>
+      <c r="G41" t="n">
+        <v>7.375</v>
+      </c>
+      <c r="H41" t="n">
+        <v>881</v>
+      </c>
+      <c r="I41" t="n">
+        <v>2752</v>
+      </c>
+      <c r="J41" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="K41" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="L41" t="n">
+        <v>0</v>
+      </c>
+      <c r="M41" t="n">
+        <v>0</v>
+      </c>
+      <c r="N41" t="n">
+        <v>116</v>
+      </c>
+      <c r="O41" t="n">
+        <v>88</v>
+      </c>
+      <c r="P41" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>2321</v>
+      </c>
+      <c r="R41" t="n">
+        <v>1632</v>
+      </c>
+      <c r="S41" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="T41" t="n">
+        <v>319.92</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>9</v>
+      </c>
+      <c r="B42" t="n">
+        <v>567.967</v>
+      </c>
+      <c r="C42" t="n">
+        <v>1.543</v>
+      </c>
+      <c r="D42" t="n">
+        <v>5355.987</v>
+      </c>
+      <c r="E42" t="n">
+        <v>12.515</v>
+      </c>
+      <c r="F42" t="n">
+        <v>4885.765</v>
+      </c>
+      <c r="G42" t="n">
+        <v>19.491</v>
+      </c>
+      <c r="H42" t="n">
+        <v>2720</v>
+      </c>
+      <c r="I42" t="n">
+        <v>8431.5</v>
+      </c>
+      <c r="J42" t="n">
+        <v>0</v>
+      </c>
+      <c r="K42" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="L42" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="M42" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N42" t="n">
+        <v>268</v>
+      </c>
+      <c r="O42" t="n">
+        <v>216</v>
+      </c>
+      <c r="P42" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>7123.5</v>
+      </c>
+      <c r="R42" t="n">
+        <v>5100</v>
+      </c>
+      <c r="S42" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="T42" t="n">
+        <v>937.67</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>11</v>
+      </c>
+      <c r="B43" t="n">
+        <v>1259.213</v>
+      </c>
+      <c r="C43" t="n">
+        <v>14.689</v>
+      </c>
+      <c r="D43" t="n">
+        <v>17933.17</v>
+      </c>
+      <c r="E43" t="n">
+        <v>39.325</v>
+      </c>
+      <c r="F43" t="n">
+        <v>16654.316</v>
+      </c>
+      <c r="G43" t="n">
+        <v>21.024</v>
+      </c>
+      <c r="H43" t="n">
+        <v>6513</v>
+      </c>
+      <c r="I43" t="n">
+        <v>20465</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0</v>
+      </c>
+      <c r="K43" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L43" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="M43" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="N43" t="n">
+        <v>600</v>
+      </c>
+      <c r="O43" t="n">
+        <v>416</v>
+      </c>
+      <c r="P43" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="Q43" t="n">
+        <v>17251.5</v>
+      </c>
+      <c r="R43" t="n">
+        <v>12328</v>
+      </c>
+      <c r="S43" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="T43" t="n">
+        <v>1893.98</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>13</v>
+      </c>
+      <c r="B44" t="n">
+        <v>2362.764</v>
+      </c>
+      <c r="C44" t="n">
+        <v>14.788</v>
+      </c>
+      <c r="D44" t="n">
+        <v>91086.458</v>
+      </c>
+      <c r="E44" t="n">
+        <v>294.36</v>
+      </c>
+      <c r="F44" t="n">
+        <v>88426.189</v>
+      </c>
+      <c r="G44" t="n">
+        <v>333.786</v>
+      </c>
+      <c r="H44" t="n">
+        <v>13619</v>
+      </c>
+      <c r="I44" t="n">
+        <v>42860.5</v>
+      </c>
+      <c r="J44" t="n">
+        <v>0</v>
+      </c>
+      <c r="K44" t="n">
+        <v>0</v>
+      </c>
+      <c r="L44" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="M44" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="N44" t="n">
+        <v>1544</v>
+      </c>
+      <c r="O44" t="n">
+        <v>700</v>
+      </c>
+      <c r="P44" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="Q44" t="n">
+        <v>35951</v>
+      </c>
+      <c r="R44" t="n">
+        <v>24272</v>
+      </c>
+      <c r="S44" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="T44" t="n">
+        <v>2934.12</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>15</v>
+      </c>
+      <c r="B45" t="n">
+        <v>4327.428</v>
+      </c>
+      <c r="C45" t="n">
+        <v>6.354</v>
+      </c>
+      <c r="D45" t="n">
+        <v>374018.692</v>
+      </c>
+      <c r="E45" t="n">
+        <v>2281.847</v>
+      </c>
+      <c r="F45" t="n">
+        <v>369142.645</v>
+      </c>
+      <c r="G45" t="n">
+        <v>2232.052</v>
+      </c>
+      <c r="H45" t="n">
+        <v>26866</v>
+      </c>
+      <c r="I45" t="n">
+        <v>91280</v>
+      </c>
+      <c r="J45" t="n">
+        <v>0</v>
+      </c>
+      <c r="K45" t="n">
+        <v>0</v>
+      </c>
+      <c r="L45" t="n">
+        <v>0</v>
+      </c>
+      <c r="M45" t="n">
+        <v>0</v>
+      </c>
+      <c r="N45" t="n">
+        <v>4828</v>
+      </c>
+      <c r="O45" t="n">
+        <v>1080</v>
+      </c>
+      <c r="P45" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="Q45" t="n">
+        <v>78034.5</v>
+      </c>
+      <c r="R45" t="n">
+        <v>46296</v>
+      </c>
+      <c r="S45" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="T45" t="n">
+        <v>6084.86</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>17</v>
+      </c>
+      <c r="B46" t="n">
+        <v>7091.082</v>
+      </c>
+      <c r="C46" t="n">
+        <v>16.417</v>
+      </c>
+      <c r="D46" t="n">
+        <v>1686327.032</v>
+      </c>
+      <c r="E46" t="n">
+        <v>3802.081</v>
+      </c>
+      <c r="F46" t="n">
+        <v>1676801.444</v>
+      </c>
+      <c r="G46" t="n">
+        <v>3778.742</v>
+      </c>
+      <c r="H46" t="n">
+        <v>54484</v>
+      </c>
+      <c r="I46" t="n">
+        <v>196438</v>
+      </c>
+      <c r="J46" t="n">
+        <v>0</v>
+      </c>
+      <c r="K46" t="n">
+        <v>0</v>
+      </c>
+      <c r="L46" t="n">
+        <v>0</v>
+      </c>
+      <c r="M46" t="n">
+        <v>0</v>
+      </c>
+      <c r="N46" t="n">
+        <v>17364</v>
+      </c>
+      <c r="O46" t="n">
+        <v>1568</v>
+      </c>
+      <c r="P46" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>173693</v>
+      </c>
+      <c r="R46" t="n">
+        <v>74788</v>
+      </c>
+      <c r="S46" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="T46" t="n">
+        <v>11420.96</v>
+      </c>
+    </row>
+    <row r="47"/>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="14">
+    <mergeCell ref="A25:S25"/>
     <mergeCell ref="A16:S16"/>
+    <mergeCell ref="A37:S37"/>
+    <mergeCell ref="A36:S36"/>
     <mergeCell ref="A14:S14"/>
+    <mergeCell ref="A38:S38"/>
     <mergeCell ref="A17:S17"/>
     <mergeCell ref="A3:S3"/>
+    <mergeCell ref="A39:S39"/>
     <mergeCell ref="A4:S4"/>
+    <mergeCell ref="A26:S26"/>
+    <mergeCell ref="A24:S24"/>
     <mergeCell ref="A2:S2"/>
     <mergeCell ref="A15:S15"/>
   </mergeCells>
@@ -1393,7 +2471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1429,6 +2507,24 @@
           <t>Qiskit: Algorithm = Shor's Order Finding Simulator = statevector_simulator</t>
         </is>
       </c>
+      <c r="B2" s="1" t="n"/>
+      <c r="C2" s="1" t="n"/>
+      <c r="D2" s="1" t="n"/>
+      <c r="E2" s="1" t="n"/>
+      <c r="F2" s="1" t="n"/>
+      <c r="G2" s="1" t="n"/>
+      <c r="H2" s="1" t="n"/>
+      <c r="I2" s="1" t="n"/>
+      <c r="J2" s="1" t="n"/>
+      <c r="K2" s="1" t="n"/>
+      <c r="L2" s="1" t="n"/>
+      <c r="M2" s="1" t="n"/>
+      <c r="N2" s="1" t="n"/>
+      <c r="O2" s="1" t="n"/>
+      <c r="P2" s="1" t="n"/>
+      <c r="Q2" s="1" t="n"/>
+      <c r="R2" s="1" t="n"/>
+      <c r="S2" s="1" t="n"/>
       <c r="T2" s="1" t="inlineStr"/>
     </row>
     <row r="3">
@@ -1437,6 +2533,24 @@
           <t>CPU: 12th Gen Intel(R) Core(TM) i9-12900 with 24 cores</t>
         </is>
       </c>
+      <c r="B3" s="1" t="n"/>
+      <c r="C3" s="1" t="n"/>
+      <c r="D3" s="1" t="n"/>
+      <c r="E3" s="1" t="n"/>
+      <c r="F3" s="1" t="n"/>
+      <c r="G3" s="1" t="n"/>
+      <c r="H3" s="1" t="n"/>
+      <c r="I3" s="1" t="n"/>
+      <c r="J3" s="1" t="n"/>
+      <c r="K3" s="1" t="n"/>
+      <c r="L3" s="1" t="n"/>
+      <c r="M3" s="1" t="n"/>
+      <c r="N3" s="1" t="n"/>
+      <c r="O3" s="1" t="n"/>
+      <c r="P3" s="1" t="n"/>
+      <c r="Q3" s="1" t="n"/>
+      <c r="R3" s="1" t="n"/>
+      <c r="S3" s="1" t="n"/>
       <c r="T3" s="1" t="inlineStr"/>
     </row>
     <row r="4">
@@ -1445,362 +2559,979 @@
           <t>Configuration: Min_Qubits = 10 Max_Qubits = 25 Skip_Qubits = 4 num_circuits = 2  QV_ = None Last_Updated = 2025-01-20 17:06:54</t>
         </is>
       </c>
+      <c r="B4" s="1" t="n"/>
+      <c r="C4" s="1" t="n"/>
+      <c r="D4" s="1" t="n"/>
+      <c r="E4" s="1" t="n"/>
+      <c r="F4" s="1" t="n"/>
+      <c r="G4" s="1" t="n"/>
+      <c r="H4" s="1" t="n"/>
+      <c r="I4" s="1" t="n"/>
+      <c r="J4" s="1" t="n"/>
+      <c r="K4" s="1" t="n"/>
+      <c r="L4" s="1" t="n"/>
+      <c r="M4" s="1" t="n"/>
+      <c r="N4" s="1" t="n"/>
+      <c r="O4" s="1" t="n"/>
+      <c r="P4" s="1" t="n"/>
+      <c r="Q4" s="1" t="n"/>
+      <c r="R4" s="1" t="n"/>
+      <c r="S4" s="1" t="n"/>
       <c r="T4" s="1" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="1" t="inlineStr">
         <is>
           <t>Number of Qubits</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="1" t="inlineStr">
         <is>
           <t>avg_creation_times (ms)</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="1" t="inlineStr">
         <is>
           <t>std_creation_times (ms)</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D5" s="1" t="inlineStr">
         <is>
           <t>avg_elapsed_times (ms)</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E5" s="1" t="inlineStr">
         <is>
           <t>std_elapsed_times (ms)</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F5" s="1" t="inlineStr">
         <is>
           <t>avg_quantum_times (ms)</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="G5" s="1" t="inlineStr">
         <is>
           <t>std_quantum_times (ms)</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="H5" s="1" t="inlineStr">
         <is>
           <t>avg_circuit_depths</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="I5" s="1" t="inlineStr">
         <is>
           <t>avg_transpiled_depths</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="J5" s="1" t="inlineStr">
         <is>
           <t>Average_Rescaled_fidelity</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="K5" s="1" t="inlineStr">
         <is>
           <t>Average_Hellinger_fidelity</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="L5" s="1" t="inlineStr">
         <is>
           <t>std_Rescaled_Fidelity</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
+      <c r="M5" s="1" t="inlineStr">
         <is>
           <t>std_hellinger_fidelity</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr">
+      <c r="N5" s="1" t="inlineStr">
         <is>
           <t>avg_1Q_algorithmic_gate_counts</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr">
+      <c r="O5" s="1" t="inlineStr">
         <is>
           <t>avg_2Q_algorithmic_gate_counts</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr">
+      <c r="P5" s="1" t="inlineStr">
         <is>
           <t>avg_xi (n2q/n1q+n2q)</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr">
+      <c r="Q5" s="1" t="inlineStr">
         <is>
           <t>avg_1Q_Transpiled_gate_counts</t>
         </is>
       </c>
-      <c r="R5" t="inlineStr">
+      <c r="R5" s="1" t="inlineStr">
         <is>
           <t>avg_2Q_Transpiled_gate_counts</t>
         </is>
       </c>
-      <c r="S5" t="inlineStr">
+      <c r="S5" s="1" t="inlineStr">
         <is>
           <t>avg_tr_xi (tr_n2q/tr_n1q+tr_n2q)</t>
         </is>
       </c>
-      <c r="T5" t="inlineStr">
+      <c r="T5" s="1" t="inlineStr">
         <is>
           <t>max_memory (MB)</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" s="1" t="n">
         <v>170.155</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6" s="1" t="n">
         <v>2.666</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6" s="1" t="n">
         <v>760.525</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6" s="1" t="n">
         <v>2.554</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6" s="1" t="n">
         <v>561.804</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6" s="1" t="n">
         <v>1.301</v>
       </c>
-      <c r="H6" t="n">
+      <c r="H6" s="1" t="n">
         <v>904</v>
       </c>
-      <c r="I6" t="n">
+      <c r="I6" s="1" t="n">
         <v>2732</v>
       </c>
-      <c r="J6" t="n">
+      <c r="J6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="K6" t="n">
+      <c r="K6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="L6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" t="n">
+      <c r="L6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="O6" t="n">
+      <c r="O6" s="1" t="n">
         <v>106</v>
       </c>
-      <c r="P6" t="n">
+      <c r="P6" s="1" t="n">
         <v>0.51</v>
       </c>
-      <c r="Q6" t="n">
+      <c r="Q6" s="1" t="n">
         <v>2226</v>
       </c>
-      <c r="R6" t="n">
+      <c r="R6" s="1" t="n">
         <v>1644</v>
       </c>
-      <c r="S6" t="n">
+      <c r="S6" s="1" t="n">
         <v>0.42</v>
       </c>
-      <c r="T6" t="n">
+      <c r="T6" s="1" t="n">
         <v>833</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7" s="1" t="n">
         <v>563.476</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7" s="1" t="n">
         <v>8.336</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7" s="1" t="n">
         <v>32455.561</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7" s="1" t="n">
         <v>126.366</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F7" s="1" t="n">
         <v>31924.923</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7" s="1" t="n">
         <v>122.238</v>
       </c>
-      <c r="H7" t="n">
+      <c r="H7" s="1" t="n">
         <v>2759</v>
       </c>
-      <c r="I7" t="n">
+      <c r="I7" s="1" t="n">
         <v>8259.5</v>
       </c>
-      <c r="J7" t="n">
+      <c r="J7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="K7" t="n">
+      <c r="K7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="L7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0</v>
-      </c>
-      <c r="N7" t="n">
+      <c r="L7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1" t="n">
         <v>211</v>
       </c>
-      <c r="O7" t="n">
+      <c r="O7" s="1" t="n">
         <v>285</v>
       </c>
-      <c r="P7" t="n">
+      <c r="P7" s="1" t="n">
         <v>0.57</v>
       </c>
-      <c r="Q7" t="n">
+      <c r="Q7" s="1" t="n">
         <v>6788.5</v>
       </c>
-      <c r="R7" t="n">
+      <c r="R7" s="1" t="n">
         <v>5130</v>
       </c>
-      <c r="S7" t="n">
+      <c r="S7" s="1" t="n">
         <v>0.43</v>
       </c>
-      <c r="T7" t="n">
+      <c r="T7" s="1" t="n">
         <v>833</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8" s="1" t="n">
         <v>1227.833</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8" s="1" t="n">
         <v>12.741</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8" s="1" t="n">
         <v>418577.785</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8" s="1" t="n">
         <v>340.93</v>
       </c>
-      <c r="F8" t="n">
+      <c r="F8" s="1" t="n">
         <v>417349.223</v>
       </c>
-      <c r="G8" t="n">
+      <c r="G8" s="1" t="n">
         <v>333.397</v>
       </c>
-      <c r="H8" t="n">
+      <c r="H8" s="1" t="n">
         <v>6478</v>
       </c>
-      <c r="I8" t="n">
+      <c r="I8" s="1" t="n">
         <v>19484</v>
       </c>
-      <c r="J8" t="n">
+      <c r="J8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="K8" t="n">
+      <c r="K8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="L8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0</v>
-      </c>
-      <c r="N8" t="n">
+      <c r="L8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" s="1" t="n">
         <v>361</v>
       </c>
-      <c r="O8" t="n">
+      <c r="O8" s="1" t="n">
         <v>588</v>
       </c>
-      <c r="P8" t="n">
+      <c r="P8" s="1" t="n">
         <v>0.62</v>
       </c>
-      <c r="Q8" t="n">
+      <c r="Q8" s="1" t="n">
         <v>15964.5</v>
       </c>
-      <c r="R8" t="n">
+      <c r="R8" s="1" t="n">
         <v>12384</v>
       </c>
-      <c r="S8" t="n">
+      <c r="S8" s="1" t="n">
         <v>0.44</v>
       </c>
-      <c r="T8" t="n">
+      <c r="T8" s="1" t="n">
         <v>1643.45</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9" s="1" t="n">
         <v>2479.225</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9" s="1" t="n">
         <v>58.466</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9" s="1" t="n">
         <v>13346085.5</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9" s="1" t="n">
         <v>4164.559</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F9" s="1" t="n">
         <v>13343574.897</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G9" s="1" t="n">
         <v>4186.765</v>
       </c>
-      <c r="H9" t="n">
+      <c r="H9" s="1" t="n">
         <v>12997</v>
       </c>
-      <c r="I9" t="n">
+      <c r="I9" s="1" t="n">
         <v>38265.5</v>
       </c>
-      <c r="J9" t="n">
+      <c r="J9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="K9" t="n">
+      <c r="K9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="L9" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N9" t="n">
+      <c r="L9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1" t="n">
         <v>551</v>
       </c>
-      <c r="O9" t="n">
+      <c r="O9" s="1" t="n">
         <v>1045</v>
       </c>
-      <c r="P9" t="n">
+      <c r="P9" s="1" t="n">
         <v>0.65</v>
       </c>
-      <c r="Q9" t="n">
+      <c r="Q9" s="1" t="n">
         <v>30840</v>
       </c>
-      <c r="R9" t="n">
+      <c r="R9" s="1" t="n">
         <v>24362</v>
       </c>
-      <c r="S9" t="n">
+      <c r="S9" s="1" t="n">
         <v>0.44</v>
       </c>
-      <c r="T9" t="n">
+      <c r="T9" s="1" t="n">
         <v>5024.67</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr"/>
+      <c r="B10" s="1" t="inlineStr"/>
+      <c r="C10" s="1" t="inlineStr"/>
+      <c r="D10" s="1" t="inlineStr"/>
+      <c r="E10" s="1" t="inlineStr"/>
+      <c r="F10" s="1" t="inlineStr"/>
+      <c r="G10" s="1" t="inlineStr"/>
+      <c r="H10" s="1" t="inlineStr"/>
+      <c r="I10" s="1" t="inlineStr"/>
+      <c r="J10" s="1" t="inlineStr"/>
+      <c r="K10" s="1" t="inlineStr"/>
+      <c r="L10" s="1" t="inlineStr"/>
+      <c r="M10" s="1" t="inlineStr"/>
+      <c r="N10" s="1" t="inlineStr"/>
+      <c r="O10" s="1" t="inlineStr"/>
+      <c r="P10" s="1" t="inlineStr"/>
+      <c r="Q10" s="1" t="inlineStr"/>
+      <c r="R10" s="1" t="inlineStr"/>
+      <c r="S10" s="1" t="inlineStr"/>
+      <c r="T10" s="1" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Qiskit: Algorithm = Shor's Order Finding Simulator = statevector_simulator</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="n"/>
+      <c r="C11" s="1" t="n"/>
+      <c r="D11" s="1" t="n"/>
+      <c r="E11" s="1" t="n"/>
+      <c r="F11" s="1" t="n"/>
+      <c r="G11" s="1" t="n"/>
+      <c r="H11" s="1" t="n"/>
+      <c r="I11" s="1" t="n"/>
+      <c r="J11" s="1" t="n"/>
+      <c r="K11" s="1" t="n"/>
+      <c r="L11" s="1" t="n"/>
+      <c r="M11" s="1" t="n"/>
+      <c r="N11" s="1" t="n"/>
+      <c r="O11" s="1" t="n"/>
+      <c r="P11" s="1" t="n"/>
+      <c r="Q11" s="1" t="n"/>
+      <c r="R11" s="1" t="n"/>
+      <c r="S11" s="1" t="n"/>
+      <c r="T11" s="1" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>CPU: 12th Gen Intel(R) Core(TM) i9-12900 with 24 cores</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="n"/>
+      <c r="C12" s="1" t="n"/>
+      <c r="D12" s="1" t="n"/>
+      <c r="E12" s="1" t="n"/>
+      <c r="F12" s="1" t="n"/>
+      <c r="G12" s="1" t="n"/>
+      <c r="H12" s="1" t="n"/>
+      <c r="I12" s="1" t="n"/>
+      <c r="J12" s="1" t="n"/>
+      <c r="K12" s="1" t="n"/>
+      <c r="L12" s="1" t="n"/>
+      <c r="M12" s="1" t="n"/>
+      <c r="N12" s="1" t="n"/>
+      <c r="O12" s="1" t="n"/>
+      <c r="P12" s="1" t="n"/>
+      <c r="Q12" s="1" t="n"/>
+      <c r="R12" s="1" t="n"/>
+      <c r="S12" s="1" t="n"/>
+      <c r="T12" s="1" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>Configuration: Min_Qubits = 7 Max_Qubits = 17 Skip_Qubits = 2 num_circuits = 2  QV_ = None Last_Updated = 2025-02-12 10:17:44</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="n"/>
+      <c r="C13" s="1" t="n"/>
+      <c r="D13" s="1" t="n"/>
+      <c r="E13" s="1" t="n"/>
+      <c r="F13" s="1" t="n"/>
+      <c r="G13" s="1" t="n"/>
+      <c r="H13" s="1" t="n"/>
+      <c r="I13" s="1" t="n"/>
+      <c r="J13" s="1" t="n"/>
+      <c r="K13" s="1" t="n"/>
+      <c r="L13" s="1" t="n"/>
+      <c r="M13" s="1" t="n"/>
+      <c r="N13" s="1" t="n"/>
+      <c r="O13" s="1" t="n"/>
+      <c r="P13" s="1" t="n"/>
+      <c r="Q13" s="1" t="n"/>
+      <c r="R13" s="1" t="n"/>
+      <c r="S13" s="1" t="n"/>
+      <c r="T13" s="1" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Number of Qubits</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>avg_creation_times (ms)</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>std_creation_times (ms)</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>avg_elapsed_times (ms)</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>std_elapsed_times (ms)</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>avg_quantum_times (ms)</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>std_quantum_times (ms)</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>avg_circuit_depths</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>avg_transpiled_depths</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Average_Rescaled_fidelity</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Average_Hellinger_fidelity</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>std_Rescaled_Fidelity</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>std_hellinger_fidelity</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>avg_1Q_algorithmic_gate_counts</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>avg_2Q_algorithmic_gate_counts</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>avg_xi (n2q/n1q+n2q)</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>avg_1Q_Transpiled_gate_counts</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>avg_2Q_Transpiled_gate_counts</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>avg_tr_xi (tr_n2q/tr_n1q+tr_n2q)</t>
+        </is>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>max_memory (MB)</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>7</v>
+      </c>
+      <c r="B15" t="n">
+        <v>192.751</v>
+      </c>
+      <c r="C15" t="n">
+        <v>8.542</v>
+      </c>
+      <c r="D15" t="n">
+        <v>263.651</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.392</v>
+      </c>
+      <c r="F15" t="n">
+        <v>116.046</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.707</v>
+      </c>
+      <c r="H15" t="n">
+        <v>881</v>
+      </c>
+      <c r="I15" t="n">
+        <v>2752</v>
+      </c>
+      <c r="J15" t="n">
+        <v>1</v>
+      </c>
+      <c r="K15" t="n">
+        <v>1</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>116</v>
+      </c>
+      <c r="O15" t="n">
+        <v>88</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>2321</v>
+      </c>
+      <c r="R15" t="n">
+        <v>1632</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="T15" t="n">
+        <v>212.59</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>9</v>
+      </c>
+      <c r="B16" t="n">
+        <v>588.256</v>
+      </c>
+      <c r="C16" t="n">
+        <v>3.775</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1651.474</v>
+      </c>
+      <c r="E16" t="n">
+        <v>76.55500000000001</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1187.42</v>
+      </c>
+      <c r="G16" t="n">
+        <v>67.11199999999999</v>
+      </c>
+      <c r="H16" t="n">
+        <v>2720</v>
+      </c>
+      <c r="I16" t="n">
+        <v>8431.5</v>
+      </c>
+      <c r="J16" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" t="n">
+        <v>1</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>268</v>
+      </c>
+      <c r="O16" t="n">
+        <v>216</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>7123.5</v>
+      </c>
+      <c r="R16" t="n">
+        <v>5100</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="T16" t="n">
+        <v>302.86</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>11</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1191.39</v>
+      </c>
+      <c r="C17" t="n">
+        <v>17.127</v>
+      </c>
+      <c r="D17" t="n">
+        <v>10934.137</v>
+      </c>
+      <c r="E17" t="n">
+        <v>134.934</v>
+      </c>
+      <c r="F17" t="n">
+        <v>9659.339</v>
+      </c>
+      <c r="G17" t="n">
+        <v>131.404</v>
+      </c>
+      <c r="H17" t="n">
+        <v>6513</v>
+      </c>
+      <c r="I17" t="n">
+        <v>20465</v>
+      </c>
+      <c r="J17" t="n">
+        <v>1</v>
+      </c>
+      <c r="K17" t="n">
+        <v>1</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" t="n">
+        <v>600</v>
+      </c>
+      <c r="O17" t="n">
+        <v>416</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>17251.5</v>
+      </c>
+      <c r="R17" t="n">
+        <v>12328</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="T17" t="n">
+        <v>456.02</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>13</v>
+      </c>
+      <c r="B18" t="n">
+        <v>2292.278</v>
+      </c>
+      <c r="C18" t="n">
+        <v>38.734</v>
+      </c>
+      <c r="D18" t="n">
+        <v>75869.266</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1.014</v>
+      </c>
+      <c r="F18" t="n">
+        <v>73351.04700000001</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="H18" t="n">
+        <v>13619</v>
+      </c>
+      <c r="I18" t="n">
+        <v>42860.5</v>
+      </c>
+      <c r="J18" t="n">
+        <v>1</v>
+      </c>
+      <c r="K18" t="n">
+        <v>1</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="n">
+        <v>1544</v>
+      </c>
+      <c r="O18" t="n">
+        <v>700</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>35951</v>
+      </c>
+      <c r="R18" t="n">
+        <v>24272</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="T18" t="n">
+        <v>711.66</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>15</v>
+      </c>
+      <c r="B19" t="n">
+        <v>4233.191</v>
+      </c>
+      <c r="C19" t="n">
+        <v>17.225</v>
+      </c>
+      <c r="D19" t="n">
+        <v>207090.61</v>
+      </c>
+      <c r="E19" t="n">
+        <v>3164.058</v>
+      </c>
+      <c r="F19" t="n">
+        <v>202222.906</v>
+      </c>
+      <c r="G19" t="n">
+        <v>3107.816</v>
+      </c>
+      <c r="H19" t="n">
+        <v>26866</v>
+      </c>
+      <c r="I19" t="n">
+        <v>91280</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.167</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.167</v>
+      </c>
+      <c r="N19" t="n">
+        <v>4828</v>
+      </c>
+      <c r="O19" t="n">
+        <v>1080</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>78034.5</v>
+      </c>
+      <c r="R19" t="n">
+        <v>46296</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="T19" t="n">
+        <v>1198.99</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>17</v>
+      </c>
+      <c r="B20" t="n">
+        <v>6653.893</v>
+      </c>
+      <c r="C20" t="n">
+        <v>70.393</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1281797.02</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1053.581</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1272304.27</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1061.368</v>
+      </c>
+      <c r="H20" t="n">
+        <v>54484</v>
+      </c>
+      <c r="I20" t="n">
+        <v>196438</v>
+      </c>
+      <c r="J20" t="n">
+        <v>1</v>
+      </c>
+      <c r="K20" t="n">
+        <v>1</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" t="n">
+        <v>17364</v>
+      </c>
+      <c r="O20" t="n">
+        <v>1568</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>173693</v>
+      </c>
+      <c r="R20" t="n">
+        <v>74788</v>
+      </c>
+      <c r="S20" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="T20" t="n">
+        <v>2225.48</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr"/>
+      <c r="Q21" t="inlineStr"/>
+      <c r="R21" t="inlineStr"/>
+      <c r="S21" t="inlineStr"/>
+      <c r="T21" t="inlineStr"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="A11:S11"/>
+    <mergeCell ref="A13:S13"/>
+    <mergeCell ref="A3:S3"/>
+    <mergeCell ref="A12:S12"/>
     <mergeCell ref="A4:S4"/>
-    <mergeCell ref="A3:S3"/>
     <mergeCell ref="A2:S2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1813,7 +3544,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T8"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2093,7 +3824,6 @@
         <v>5478.98</v>
       </c>
     </row>
-    <row r="8"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A4:S4"/>
@@ -2110,7 +3840,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T8"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2146,24 +3876,6 @@
           <t>Qiskit: Algorithm = Shor's Order Finding Simulator = fake_guadalupe-1.2.15</t>
         </is>
       </c>
-      <c r="B2" s="1" t="n"/>
-      <c r="C2" s="1" t="n"/>
-      <c r="D2" s="1" t="n"/>
-      <c r="E2" s="1" t="n"/>
-      <c r="F2" s="1" t="n"/>
-      <c r="G2" s="1" t="n"/>
-      <c r="H2" s="1" t="n"/>
-      <c r="I2" s="1" t="n"/>
-      <c r="J2" s="1" t="n"/>
-      <c r="K2" s="1" t="n"/>
-      <c r="L2" s="1" t="n"/>
-      <c r="M2" s="1" t="n"/>
-      <c r="N2" s="1" t="n"/>
-      <c r="O2" s="1" t="n"/>
-      <c r="P2" s="1" t="n"/>
-      <c r="Q2" s="1" t="n"/>
-      <c r="R2" s="1" t="n"/>
-      <c r="S2" s="1" t="n"/>
       <c r="T2" s="1" t="inlineStr"/>
     </row>
     <row r="3">
@@ -2172,24 +3884,6 @@
           <t>CPU: 12th Gen Intel(R) Core(TM) i9-12900 with 24 cores</t>
         </is>
       </c>
-      <c r="B3" s="1" t="n"/>
-      <c r="C3" s="1" t="n"/>
-      <c r="D3" s="1" t="n"/>
-      <c r="E3" s="1" t="n"/>
-      <c r="F3" s="1" t="n"/>
-      <c r="G3" s="1" t="n"/>
-      <c r="H3" s="1" t="n"/>
-      <c r="I3" s="1" t="n"/>
-      <c r="J3" s="1" t="n"/>
-      <c r="K3" s="1" t="n"/>
-      <c r="L3" s="1" t="n"/>
-      <c r="M3" s="1" t="n"/>
-      <c r="N3" s="1" t="n"/>
-      <c r="O3" s="1" t="n"/>
-      <c r="P3" s="1" t="n"/>
-      <c r="Q3" s="1" t="n"/>
-      <c r="R3" s="1" t="n"/>
-      <c r="S3" s="1" t="n"/>
       <c r="T3" s="1" t="inlineStr"/>
     </row>
     <row r="4">
@@ -2198,24 +3892,6 @@
           <t>Configuration: Min_Qubits = 10 Max_Qubits = 16 Skip_Qubits = 4 num_circuits = 2  QV_ = 32 Last_Updated = 2025-02-11 12:41:02</t>
         </is>
       </c>
-      <c r="B4" s="1" t="n"/>
-      <c r="C4" s="1" t="n"/>
-      <c r="D4" s="1" t="n"/>
-      <c r="E4" s="1" t="n"/>
-      <c r="F4" s="1" t="n"/>
-      <c r="G4" s="1" t="n"/>
-      <c r="H4" s="1" t="n"/>
-      <c r="I4" s="1" t="n"/>
-      <c r="J4" s="1" t="n"/>
-      <c r="K4" s="1" t="n"/>
-      <c r="L4" s="1" t="n"/>
-      <c r="M4" s="1" t="n"/>
-      <c r="N4" s="1" t="n"/>
-      <c r="O4" s="1" t="n"/>
-      <c r="P4" s="1" t="n"/>
-      <c r="Q4" s="1" t="n"/>
-      <c r="R4" s="1" t="n"/>
-      <c r="S4" s="1" t="n"/>
       <c r="T4" s="1" t="inlineStr"/>
     </row>
     <row r="5">
@@ -2443,28 +4119,6 @@
       <c r="T7" t="n">
         <v>497.26</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="inlineStr"/>
-      <c r="S8" t="inlineStr"/>
-      <c r="T8" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>